<commit_message>
DONE WITH DATA MANIP
</commit_message>
<xml_diff>
--- a/Data/TournamentSeedsNumbers.xlsx
+++ b/Data/TournamentSeedsNumbers.xlsx
@@ -420,7 +420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1808,7 +1810,7 @@
       <c r="A126" s="2">
         <v>2015</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B126">
         <v>1412</v>
       </c>
       <c r="C126" s="2">

</xml_diff>